<commit_message>
add names for week of 3/16
</commit_message>
<xml_diff>
--- a/temp-newnames.xlsx
+++ b/temp-newnames.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\fewapo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEB46EF-68E7-4050-A593-F7C7AF944916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC80E64E-C6F9-4339-80FF-171164E99950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{31A1FEC2-9A16-4132-85F3-F6FDF7C02A4E}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="19185" windowHeight="10200" xr2:uid="{31A1FEC2-9A16-4132-85F3-F6FDF7C02A4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="172">
   <si>
     <t>Deputies responded to a 5:47 p.m. call about a “suspicious vehicle” in a parking lot, according to investigators.  When deputies arrived on the scene at 5:51 p.m., they reportedly contacted the person in the vehicle, and at 5:56 p.m., deputies radioed that shots had been fired.</t>
   </si>
@@ -465,12 +464,108 @@
   <si>
     <t>Chehalis</t>
   </si>
+  <si>
+    <t>19000 blk of Pacific Ave So</t>
+  </si>
+  <si>
+    <t>Spanaway</t>
+  </si>
+  <si>
+    <t>Jeremy Darryl Dayton</t>
+  </si>
+  <si>
+    <t>The victim was being sought on a warrant for second-degree assault when the South Sound Gang Task Force located him.  The Pierce Co Sheriff's office called in the SWAT to assist with the arrest.  Police allege there was an exchange of gunfire; two deputies were shot, in addition to the victim.</t>
+  </si>
+  <si>
+    <t>https://www.thenewstribune.com/news/local/crime/article259446764.html</t>
+  </si>
+  <si>
+    <t>https://www.q13fox.com/news/2-swat-officers-shot-in-spanaway-pierce-county-sheriffs-department-says</t>
+  </si>
+  <si>
+    <t>3600 South Findley Street</t>
+  </si>
+  <si>
+    <t>Three men allegedly robbed a Cannabis store in Bellevue at gunpoint.  They were chased from Bellevue to Seattle, where their vehicle lost a wheel.  Two were apprehended, the third fled and allegedly fired at officers when they tracked him down to a shed.  They returned fire, killing him.</t>
+  </si>
+  <si>
+    <t>4200 block of Pine Street</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>9600 pacific avenue</t>
+  </si>
+  <si>
+    <t>https://komonews.com/news/local/pierce-county-car-chase-ends-fatally-as-suspect-faces-vehicular-homicide-charge</t>
+  </si>
+  <si>
+    <t>https://www.kiro7.com/news/local/police-shoot-kill-man-near-tacoma-mall/63VCCJOXINBG7KIVQ7D5JLYFLM/</t>
+  </si>
+  <si>
+    <t>A man was shot in the middle of the street within 5 seconds of police arrival.  Unclear if he was armed, but police allege that he was.</t>
+  </si>
+  <si>
+    <t>6th Ave and W Lewis St</t>
+  </si>
+  <si>
+    <t>Pasco</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Pasco Police Department</t>
+  </si>
+  <si>
+    <t>https://www.yaktrinews.com/siu-identifies-late-homicide-suspect-pasco-police-officers-who-shot-him-2/</t>
+  </si>
+  <si>
+    <t>Officers responded to 911 call reporting  a physical altercation.  When they arrived, they found one man had been stabbed and killed.  They located a man armed with a knife, but he is alleged to have threatened them with the weapon, which led them to shoot him.</t>
+  </si>
+  <si>
+    <t>Mauricio Martinez Yanez</t>
+  </si>
+  <si>
+    <t>https://www.seattletimes.com/seattle-news/law-justice/seattle-police-release-video-and-timeline-of-fatal-shooting-of-bellevue-pot-shop-robbery-suspect/</t>
+  </si>
+  <si>
+    <t>Deputies tried to stop a car that was driving recklessly.  The driver fled, crashing into another car and killing the passenger in that car, as well as injuring the driver of that car, and a passenger in his car.</t>
+  </si>
+  <si>
+    <t>David A. Babcock</t>
+  </si>
+  <si>
+    <t>Sedro-Woolley</t>
+  </si>
+  <si>
+    <t>https://www.cascadiadaily.com/news/2022/mar/12/protest-for-david-babcock-gathers-outside-sedro-woolley-police-department/</t>
+  </si>
+  <si>
+    <t>Sedro-Woolley Police Department</t>
+  </si>
+  <si>
+    <t>Fruitdale Road and McGargile Road</t>
+  </si>
+  <si>
+    <t>Skagit</t>
+  </si>
+  <si>
+    <t>Police pursued a "possibly stolen vehicle".  When the driver sought to elude a set of spike strips, he was shot in the back of the head.</t>
+  </si>
+  <si>
+    <t>Unarmed</t>
+  </si>
+  <si>
+    <t>Gabriel Artz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,6 +633,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0F1419"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -560,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -588,6 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -903,17 +1005,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F0DBCB-9121-4F5F-8ACA-ADE3728A546C}">
-  <dimension ref="A1:AO13"/>
+  <dimension ref="A1:AO19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1044,7 +1147,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>900001</v>
+        <v>90001</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>30</v>
@@ -1121,7 +1224,8 @@
     </row>
     <row r="3" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
-        <v>900002</v>
+        <f>A2+1</f>
+        <v>90002</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="15" t="s">
@@ -1178,7 +1282,8 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>900003</v>
+        <f t="shared" ref="A4:A19" si="0">A3+1</f>
+        <v>90003</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
@@ -1261,7 +1366,8 @@
     </row>
     <row r="5" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
-        <v>900004</v>
+        <f t="shared" si="0"/>
+        <v>90004</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>70</v>
@@ -1323,7 +1429,8 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>900005</v>
+        <f t="shared" si="0"/>
+        <v>90005</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>14</v>
@@ -1406,7 +1513,8 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>900006</v>
+        <f t="shared" si="0"/>
+        <v>90006</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>97</v>
@@ -1485,7 +1593,8 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>900007</v>
+        <f t="shared" si="0"/>
+        <v>90007</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>69</v>
@@ -1562,7 +1671,8 @@
     </row>
     <row r="9" spans="1:41" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>900008</v>
+        <f t="shared" si="0"/>
+        <v>90008</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="18"/>
@@ -1616,15 +1726,16 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>900009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
+        <f t="shared" si="0"/>
+        <v>90009</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="C10" s="18">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>13</v>
@@ -1636,66 +1747,62 @@
         <v>80</v>
       </c>
       <c r="I10" s="14">
-        <v>44610</v>
+        <v>44608</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="M10">
-        <v>98532</v>
+        <v>98284</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="O10" s="4"/>
       <c r="P10">
-        <v>46.661088499999998</v>
+        <v>48.521746</v>
       </c>
       <c r="Q10">
-        <v>-122.966494</v>
+        <v>-122.2128101</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="V10" t="s">
-        <v>132</v>
-      </c>
-      <c r="W10" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="Y10" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>83</v>
+        <v>126</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="AD10" s="4" t="s">
         <v>136</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>900010</v>
+        <f t="shared" si="0"/>
+        <v>90010</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="C11" s="18">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>13</v>
@@ -1707,31 +1814,34 @@
         <v>80</v>
       </c>
       <c r="I11" s="14">
-        <v>44616</v>
+        <v>44610</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="M11">
-        <v>98402</v>
-      </c>
-      <c r="N11" t="s">
-        <v>3</v>
+        <v>98532</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="P11">
-        <v>47.253778599999997</v>
+        <v>46.661088499999998</v>
       </c>
       <c r="Q11">
-        <v>-122.4377159</v>
+        <v>-122.966494</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>1</v>
@@ -1740,33 +1850,31 @@
         <v>132</v>
       </c>
       <c r="W11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y11" t="s">
         <v>129</v>
       </c>
       <c r="AB11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AD11" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AE11" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>122</v>
+      <c r="AE11" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>900011</v>
+        <f t="shared" si="0"/>
+        <v>90011</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C12" s="18">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>13</v>
@@ -1778,34 +1886,31 @@
         <v>80</v>
       </c>
       <c r="I12" s="14">
-        <v>44625</v>
-      </c>
-      <c r="J12" t="s">
-        <v>108</v>
+        <v>44616</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="M12">
-        <v>98104</v>
+        <v>98402</v>
       </c>
       <c r="N12" t="s">
-        <v>110</v>
-      </c>
-      <c r="O12" t="s">
-        <v>109</v>
+        <v>3</v>
       </c>
       <c r="P12">
-        <v>47.604594800000001</v>
+        <v>47.253778599999997</v>
       </c>
       <c r="Q12">
-        <v>-122.3376505</v>
+        <v>-122.4377159</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>1</v>
@@ -1814,85 +1919,460 @@
         <v>132</v>
       </c>
       <c r="W12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Y12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AB12" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>136</v>
       </c>
       <c r="AE12" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>900012</v>
+        <f t="shared" si="0"/>
+        <v>90012</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="20">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="C13" s="18">
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
       <c r="I13" s="14">
-        <v>44626</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="K13" t="s">
-        <v>114</v>
-      </c>
-      <c r="L13" t="s">
+        <v>44625</v>
+      </c>
+      <c r="J13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="M13">
-        <v>98032</v>
+        <v>98104</v>
       </c>
       <c r="N13" t="s">
         <v>110</v>
       </c>
+      <c r="O13" t="s">
+        <v>109</v>
+      </c>
       <c r="P13">
+        <v>47.604594800000001</v>
+      </c>
+      <c r="Q13">
+        <v>-122.3376505</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" t="s">
+        <v>132</v>
+      </c>
+      <c r="W13" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>90013</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="20">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="14">
+        <v>44626</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>98032</v>
+      </c>
+      <c r="N14" t="s">
+        <v>110</v>
+      </c>
+      <c r="P14">
         <v>47.358430499999997</v>
       </c>
-      <c r="Q13">
+      <c r="Q14">
         <v>-122.2984202</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="S14" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Y14" t="s">
         <v>127</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AB14" t="s">
         <v>117</v>
       </c>
-      <c r="AD13" s="4" t="s">
+      <c r="AD14" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="AE13" s="13" t="s">
+      <c r="AE14" s="13" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>90014</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="20">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="14">
+        <v>44633</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>99301</v>
+      </c>
+      <c r="N15" t="s">
+        <v>156</v>
+      </c>
+      <c r="P15">
+        <v>46.229645300000001</v>
+      </c>
+      <c r="Q15">
+        <v>-119.0980397</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE15" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>90015</v>
+      </c>
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="14">
+        <v>44635</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="K16" t="s">
+        <v>141</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>98387</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>47.084417000000002</v>
+      </c>
+      <c r="Q16">
+        <v>-122.4373025</v>
+      </c>
+      <c r="R16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL16" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>90016</v>
+      </c>
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="14">
+        <v>44636</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K17" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>98118</v>
+      </c>
+      <c r="N17" t="s">
+        <v>110</v>
+      </c>
+      <c r="P17">
+        <v>47.551982700000003</v>
+      </c>
+      <c r="Q17">
+        <v>-122.2904632</v>
+      </c>
+      <c r="R17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD17" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>90017</v>
+      </c>
+      <c r="C18">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="14">
+        <v>44636</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K18" t="s">
+        <v>86</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>98409</v>
+      </c>
+      <c r="N18" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>47.218786399999999</v>
+      </c>
+      <c r="Q18">
+        <v>-122.47634600000001</v>
+      </c>
+      <c r="R18" t="s">
+        <v>87</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>90018</v>
+      </c>
+      <c r="C19">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" s="14">
+        <v>44636</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>98444</v>
+      </c>
+      <c r="N19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>47.169878199999999</v>
+      </c>
+      <c r="Q19">
+        <v>-122.4366663</v>
+      </c>
+      <c r="R19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AE6" r:id="rId1" xr:uid="{D03245A1-3E52-4EC0-A18E-5504B1C93CB2}"/>
     <hyperlink ref="AE8" r:id="rId2" xr:uid="{D7911B47-3EF0-4011-8CE3-EA4924370F80}"/>
-    <hyperlink ref="AE10" r:id="rId3" xr:uid="{B73FD268-71E1-489A-B845-36AE717295E6}"/>
-    <hyperlink ref="AE13" r:id="rId4" xr:uid="{A5BDE563-C8A4-4315-B2BF-E31956FC5DB7}"/>
+    <hyperlink ref="AE11" r:id="rId3" xr:uid="{B73FD268-71E1-489A-B845-36AE717295E6}"/>
+    <hyperlink ref="AE14" r:id="rId4" xr:uid="{A5BDE563-C8A4-4315-B2BF-E31956FC5DB7}"/>
+    <hyperlink ref="AL16" r:id="rId5" xr:uid="{4490D4D0-B384-4F02-AFC7-3758D012F081}"/>
+    <hyperlink ref="AE10" r:id="rId6" xr:uid="{4EA5E7F5-D068-4D68-9489-22E9C8CCE60D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>